<commit_message>
Solved Problem Links must have an p_nom_extendable
</commit_message>
<xml_diff>
--- a/data/Setup.xlsx
+++ b/data/Setup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fichtnergmbh-my.sharepoint.com/personal/flaizd_fis_fichtnergroup_com/Documents/Masterarbeit/Repository/Master-Thesis/OPTIMIZER/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="586" documentId="8_{6AEDBBA3-4D35-4A2A-8A1D-E5BF92F27C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1FB7F1F-490C-4F64-9655-FEC6AAB94464}"/>
+  <xr:revisionPtr revIDLastSave="681" documentId="8_{6AEDBBA3-4D35-4A2A-8A1D-E5BF92F27C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D135D8DB-5AC1-473D-94CD-E2F881E7CF4C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" firstSheet="2" activeTab="7" xr2:uid="{2C9D1742-10EB-41B0-B231-58DC9394551A}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{2C9D1742-10EB-41B0-B231-58DC9394551A}"/>
   </bookViews>
   <sheets>
     <sheet name="CST" sheetId="12" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="325">
   <si>
     <t>name</t>
   </si>
@@ -1055,34 +1055,16 @@
     <t>$/kWh</t>
   </si>
   <si>
-    <t>link5</t>
-  </si>
-  <si>
     <t>link0</t>
   </si>
   <si>
-    <t>bus1 solar</t>
+    <t>Demand 1</t>
   </si>
   <si>
-    <t>bus2 solar</t>
+    <t>Store</t>
   </si>
   <si>
-    <t>bus3 solar</t>
-  </si>
-  <si>
-    <t>bus3 fossil</t>
-  </si>
-  <si>
-    <t>solar heat</t>
-  </si>
-  <si>
-    <t>fossil heat</t>
-  </si>
-  <si>
-    <t>TES</t>
-  </si>
-  <si>
-    <t>Load</t>
+    <t>bus3</t>
   </si>
 </sst>
 </file>
@@ -1157,12 +1139,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1189,7 +1177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1218,6 +1206,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1273,7 +1262,7 @@
   <autoFilter ref="A7:G180" xr:uid="{A1A8C0EC-B48A-4A18-B217-C0EB14485B01}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Loads"/>
+        <filter val="Links"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1671,7 +1660,7 @@
   <dimension ref="A1:B8761"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1682,7 +1671,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="str">
         <f>generators!A2</f>
@@ -71781,7 +71770,7 @@
   </sheetPr>
   <dimension ref="A1:N180"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
@@ -71798,15 +71787,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -71816,13 +71805,13 @@
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -71832,13 +71821,13 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -71848,13 +71837,13 @@
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
@@ -71864,13 +71853,13 @@
       <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -71880,13 +71869,13 @@
       <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
@@ -73636,7 +73625,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>178</v>
       </c>
@@ -73659,7 +73648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>178</v>
       </c>
@@ -73682,7 +73671,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>178</v>
       </c>
@@ -73705,7 +73694,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>178</v>
       </c>
@@ -73728,7 +73717,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>178</v>
       </c>
@@ -73751,7 +73740,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>178</v>
       </c>
@@ -73772,7 +73761,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>178</v>
       </c>
@@ -73795,7 +73784,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>178</v>
       </c>
@@ -73818,7 +73807,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>178</v>
       </c>
@@ -73841,7 +73830,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>178</v>
       </c>
@@ -73864,7 +73853,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>178</v>
       </c>
@@ -73887,7 +73876,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>178</v>
       </c>
@@ -73910,7 +73899,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>178</v>
       </c>
@@ -73933,7 +73922,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>178</v>
       </c>
@@ -73956,7 +73945,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>178</v>
       </c>
@@ -73979,7 +73968,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>178</v>
       </c>
@@ -74002,7 +73991,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>178</v>
       </c>
@@ -74025,7 +74014,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>178</v>
       </c>
@@ -74048,7 +74037,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>178</v>
       </c>
@@ -74071,7 +74060,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>178</v>
       </c>
@@ -74094,7 +74083,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>178</v>
       </c>
@@ -74117,7 +74106,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>178</v>
       </c>
@@ -74140,7 +74129,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>178</v>
       </c>
@@ -74163,7 +74152,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>178</v>
       </c>
@@ -74186,7 +74175,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>178</v>
       </c>
@@ -74209,7 +74198,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>178</v>
       </c>
@@ -74232,7 +74221,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>178</v>
       </c>
@@ -74255,7 +74244,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>178</v>
       </c>
@@ -74278,7 +74267,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>178</v>
       </c>
@@ -74301,7 +74290,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>178</v>
       </c>
@@ -74324,7 +74313,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>178</v>
       </c>
@@ -74347,7 +74336,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>178</v>
       </c>
@@ -74370,7 +74359,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>178</v>
       </c>
@@ -74393,7 +74382,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>178</v>
       </c>
@@ -74416,7 +74405,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>178</v>
       </c>
@@ -74439,7 +74428,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>178</v>
       </c>
@@ -74462,7 +74451,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>178</v>
       </c>
@@ -74485,7 +74474,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>178</v>
       </c>
@@ -74508,7 +74497,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>178</v>
       </c>
@@ -74531,7 +74520,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>178</v>
       </c>
@@ -74554,7 +74543,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>178</v>
       </c>
@@ -74577,7 +74566,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>178</v>
       </c>
@@ -74600,7 +74589,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>216</v>
       </c>
@@ -74623,7 +74612,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>216</v>
       </c>
@@ -74646,7 +74635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>216</v>
       </c>
@@ -74669,7 +74658,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>216</v>
       </c>
@@ -74692,7 +74681,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>216</v>
       </c>
@@ -74715,7 +74704,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>216</v>
       </c>
@@ -74738,7 +74727,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>216</v>
       </c>
@@ -74761,7 +74750,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>216</v>
       </c>
@@ -74784,7 +74773,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>216</v>
       </c>
@@ -74807,7 +74796,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>216</v>
       </c>
@@ -75983,10 +75972,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76001,34 +75990,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>323</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>324</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B4" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>326</v>
-      </c>
-      <c r="B5" t="s">
-        <v>328</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -76041,10 +76022,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76052,36 +76033,14 @@
     <col min="1" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="B3" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -76094,10 +76053,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76105,7 +76064,7 @@
     <col min="1" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -76124,45 +76083,63 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>323</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>287</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1">
         <v>550000</v>
       </c>
       <c r="E2" s="1">
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>313</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>287</v>
       </c>
       <c r="D3" s="1">
-        <v>300000</v>
+        <v>600000</v>
       </c>
       <c r="E3" s="1">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="F3" t="s">
-        <v>328</v>
+        <v>8</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -76195,10 +76172,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76206,7 +76183,7 @@
     <col min="1" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -76219,47 +76196,51 @@
       <c r="D1" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>323</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>324</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="1">
+        <v>100</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>325</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
+      <c r="E3" s="1">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -76275,8 +76256,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76297,13 +76278,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -76316,10 +76297,10 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76329,7 +76310,7 @@
     <col min="6" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -76345,11 +76326,14 @@
       <c r="E1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -76357,15 +76341,18 @@
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>324</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>287</v>
       </c>
     </row>

</xml_diff>